<commit_message>
declaracion de esfuerzo corregida
</commit_message>
<xml_diff>
--- a/Docs/DeclaracionEsfuerzo.xlsx
+++ b/Docs/DeclaracionEsfuerzo.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Nota global de experimento</t>
   </si>
@@ -546,7 +546,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,9 +590,7 @@
       <c r="G3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="6">
-        <v>3.8</v>
-      </c>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -610,10 +608,10 @@
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="5">
-        <v>25</v>
+        <v>33.332999999999998</v>
       </c>
       <c r="H4" s="6">
-        <v>3.8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -632,32 +630,24 @@
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="5">
-        <v>25</v>
+        <v>33.332999999999998</v>
       </c>
       <c r="H5" s="6">
-        <v>3.8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="7" t="s">
-        <v>3</v>
-      </c>
+      <c r="D6" s="7"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="5">
-        <v>25</v>
-      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="5"/>
       <c r="H6" s="6">
-        <v>3.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -676,10 +666,10 @@
         <v>3</v>
       </c>
       <c r="G7" s="5">
-        <v>25</v>
+        <v>33.332999999999998</v>
       </c>
       <c r="H7" s="6">
-        <v>3.8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -691,7 +681,9 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="G8" s="7">
+        <v>100</v>
+      </c>
       <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>